<commit_message>
modified data model and SQA Checklist
</commit_message>
<xml_diff>
--- a/Documentation/QUALITY/SQA Checklist.xlsx
+++ b/Documentation/QUALITY/SQA Checklist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>Task ID</t>
   </si>
@@ -200,13 +200,34 @@
   </si>
   <si>
     <t>---</t>
+  </si>
+  <si>
+    <t>System Development</t>
+  </si>
+  <si>
+    <t>Project Analysis</t>
+  </si>
+  <si>
+    <t>ETL Process</t>
+  </si>
+  <si>
+    <t>Project Team</t>
+  </si>
+  <si>
+    <t>Project Developers</t>
+  </si>
+  <si>
+    <t>5 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +272,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,7 +289,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -303,22 +332,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -330,7 +348,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -351,22 +368,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -379,6 +386,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,45 +708,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A27" activeCellId="3" sqref="A24:XFD24 A25:XFD25 A26:XFD26 A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="58.28515625" customWidth="1"/>
-    <col min="4" max="9" width="18.7109375" customWidth="1"/>
+    <col min="4" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -725,7 +776,7 @@
       <c r="I3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -734,20 +785,20 @@
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="5">
+      <c r="E4" s="19">
         <v>42752</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="19">
         <v>42752</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="4"/>
       <c r="K4" t="s">
         <v>11</v>
@@ -758,22 +809,22 @@
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="19">
         <v>42752</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="19">
         <v>42752</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>1</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="4"/>
       <c r="K5" t="s">
         <v>12</v>
@@ -784,22 +835,22 @@
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="19">
         <v>42752</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="19">
         <v>42752</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="6" t="s">
         <v>55</v>
       </c>
       <c r="I6" s="4"/>
@@ -812,22 +863,22 @@
         <v>4</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="19">
         <v>42755</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="19">
         <v>42755</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>3</v>
       </c>
       <c r="I7" s="4"/>
@@ -840,22 +891,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="19">
         <v>42768</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="19">
         <v>42768</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>1</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="6">
         <v>4</v>
       </c>
       <c r="I8" s="4"/>
@@ -868,20 +919,20 @@
         <v>6</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="5">
+      <c r="E9" s="19">
         <v>42775</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>0.2</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -889,22 +940,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="19">
         <v>42776</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="19">
         <v>42776</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>1</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="4"/>
       <c r="K10" t="s">
         <v>16</v>
@@ -915,462 +966,511 @@
         <v>8</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="19">
         <v>42776</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="19">
         <v>42777</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>1</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>7</v>
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+    <row r="12" spans="1:11" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>9</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="5">
-        <v>42780</v>
-      </c>
-      <c r="F12" s="5">
-        <v>42780</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-      <c r="H12" s="7">
-        <v>3</v>
-      </c>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>10</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="5">
-        <v>42781</v>
-      </c>
-      <c r="F13" s="5">
-        <v>42781</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="7">
-        <v>9</v>
-      </c>
-      <c r="I13" s="4"/>
+      <c r="E13" s="19">
+        <v>42780</v>
+      </c>
+      <c r="F13" s="19">
+        <v>42780</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>3</v>
+      </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="12" t="s">
-        <v>31</v>
+      <c r="C14" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="5">
-        <v>42782</v>
-      </c>
-      <c r="F14" s="5">
-        <v>42782</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1</v>
-      </c>
-      <c r="H14" s="7">
+      <c r="E14" s="19">
+        <v>42781</v>
+      </c>
+      <c r="F14" s="19">
+        <v>42781</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="6">
         <v>9</v>
       </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="19">
+        <v>42782</v>
+      </c>
+      <c r="F15" s="19">
+        <v>42782</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <v>9</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="14" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="D16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="19">
         <v>42781</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F16" s="19">
         <v>42781</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G16" s="5">
         <v>1</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H16" s="6">
         <v>9</v>
       </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>13</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="5">
-        <v>42782</v>
-      </c>
-      <c r="F16" s="5">
-        <v>42783</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>14</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="5">
-        <v>42784</v>
-      </c>
-      <c r="F17" s="5">
-        <v>42786</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>57</v>
+      <c r="E17" s="19">
+        <v>42782</v>
+      </c>
+      <c r="F17" s="19">
+        <v>42783</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="12" t="s">
-        <v>37</v>
+      <c r="C18" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="5">
-        <v>42787</v>
-      </c>
-      <c r="F18" s="5">
-        <v>42790</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7">
-        <v>14</v>
+        <v>53</v>
+      </c>
+      <c r="E18" s="19">
+        <v>42784</v>
+      </c>
+      <c r="F18" s="19">
+        <v>42786</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="15" t="s">
-        <v>36</v>
+      <c r="C19" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E19" s="19">
-        <v>42791</v>
-      </c>
-      <c r="F19" s="5">
-        <v>42794</v>
+        <v>42787</v>
+      </c>
+      <c r="F19" s="19">
+        <v>42790</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="7">
-        <v>15</v>
+      <c r="H19" s="6">
+        <v>14</v>
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>17</v>
-      </c>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="13" t="s">
-        <v>38</v>
+      <c r="C20" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="5">
+        <v>65</v>
+      </c>
+      <c r="E20" s="19">
+        <v>42790</v>
+      </c>
+      <c r="F20" s="19">
         <v>42796</v>
       </c>
-      <c r="F20" s="5">
-        <v>42796</v>
-      </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="H20" s="6"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="5">
-        <v>42796</v>
-      </c>
-      <c r="F21" s="5">
-        <v>42796</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="4"/>
+    <row r="21" spans="1:9" s="27" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="33" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="12" t="s">
-        <v>39</v>
+      <c r="C22" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="5">
-        <v>42798</v>
-      </c>
-      <c r="F22" s="5">
-        <v>42798</v>
+        <v>54</v>
+      </c>
+      <c r="E22" s="19">
+        <v>42791</v>
+      </c>
+      <c r="F22" s="19">
+        <v>42794</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="7">
-        <v>18</v>
+      <c r="H22" s="6">
+        <v>15</v>
       </c>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="19">
+        <v>42796</v>
+      </c>
+      <c r="F23" s="19">
+        <v>42796</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="19">
+        <v>42796</v>
+      </c>
+      <c r="F24" s="19">
+        <v>42796</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="19">
+        <v>42798</v>
+      </c>
+      <c r="F25" s="19">
+        <v>42798</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="6">
+        <v>18</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="5">
+      <c r="D26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="19">
         <v>42798</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F26" s="19">
         <v>42798</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7">
+      <c r="G26" s="4"/>
+      <c r="H26" s="6">
         <v>19</v>
       </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>21</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="16" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="20">
+      <c r="D27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="20">
         <v>42800</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F27" s="20">
         <v>42800</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9">
+      <c r="G27" s="7"/>
+      <c r="H27" s="8">
         <v>20</v>
       </c>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>22</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="17" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="20">
+      <c r="D28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="20">
         <v>42801</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F28" s="20">
         <v>42801</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9">
+      <c r="G28" s="7"/>
+      <c r="H28" s="8">
         <v>21</v>
       </c>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>23</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="17" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="20">
+      <c r="D29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="20">
         <v>42801</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F29" s="20">
         <v>42801</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9">
+      <c r="G29" s="7"/>
+      <c r="H29" s="8">
         <v>22</v>
       </c>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>24</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="16" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E30" s="20">
         <v>42803</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F30" s="20">
         <v>42805</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9">
+      <c r="G30" s="7"/>
+      <c r="H30" s="8">
         <v>15</v>
       </c>
-      <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>25</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="17" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E31" s="19">
         <v>42807</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F31" s="19">
         <v>42808</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="7">
+      <c r="G31" s="4"/>
+      <c r="H31" s="6">
         <v>24</v>
       </c>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>26</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="18" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E32" s="19">
         <v>42810</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F32" s="19">
         <v>42812</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="7">
+      <c r="G32" s="4"/>
+      <c r="H32" s="6">
         <v>16</v>
       </c>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>27</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="18" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1400,42 +1500,42 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move files to midterm folder
</commit_message>
<xml_diff>
--- a/Documentation/QUALITY/SQA Checklist.xlsx
+++ b/Documentation/QUALITY/SQA Checklist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>Task ID</t>
   </si>
@@ -130,42 +130,6 @@
     <t>Identify possible solutions</t>
   </si>
   <si>
-    <t>Business Intelligence Tool</t>
-  </si>
-  <si>
-    <t>Login/Register Interface</t>
-  </si>
-  <si>
-    <t>Advisory form</t>
-  </si>
-  <si>
-    <t>LGU basic information form</t>
-  </si>
-  <si>
-    <t>Request supply form</t>
-  </si>
-  <si>
-    <t>List of accounts grid view</t>
-  </si>
-  <si>
-    <t>List of requests grid view</t>
-  </si>
-  <si>
-    <t>Historical data form</t>
-  </si>
-  <si>
-    <t>Add and update data</t>
-  </si>
-  <si>
-    <t>Working Business Intelligence tool</t>
-  </si>
-  <si>
-    <t>Working database</t>
-  </si>
-  <si>
-    <t>Complete proof of concept for system</t>
-  </si>
-  <si>
     <t>Project Management Plan</t>
   </si>
   <si>
@@ -193,9 +157,6 @@
     <t>9 , 10, 11, 12, 13</t>
   </si>
   <si>
-    <t>15, 16</t>
-  </si>
-  <si>
     <t>---</t>
   </si>
   <si>
@@ -205,19 +166,31 @@
     <t>Project Analysis</t>
   </si>
   <si>
-    <t>ETL Process</t>
-  </si>
-  <si>
     <t>Project Team</t>
   </si>
   <si>
     <t>Project Developers</t>
   </si>
   <si>
-    <t>5 days</t>
-  </si>
-  <si>
     <t>Database Design</t>
+  </si>
+  <si>
+    <t>Change of Scope</t>
+  </si>
+  <si>
+    <t>Analyze new system process</t>
+  </si>
+  <si>
+    <t>System Design</t>
+  </si>
+  <si>
+    <t>Implement Business Intelligence Tool</t>
+  </si>
+  <si>
+    <t>Data Warehousing Process</t>
+  </si>
+  <si>
+    <t>End-user Web Application</t>
   </si>
 </sst>
 </file>
@@ -289,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -332,11 +305,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -428,6 +412,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +801,7 @@
         <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E5" s="15">
         <v>42752</v>
@@ -839,7 +827,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E6" s="15">
         <v>42752</v>
@@ -851,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="I6" s="4"/>
       <c r="K6" t="s">
@@ -867,7 +855,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E7" s="15">
         <v>42755</v>
@@ -892,10 +880,10 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E8" s="15">
         <v>42768</v>
@@ -920,14 +908,14 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="11" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="15">
         <v>42775</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="G9" s="5">
         <v>0.2</v>
@@ -941,10 +929,10 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E10" s="15">
         <v>42776</v>
@@ -970,7 +958,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E11" s="15">
         <v>42776</v>
@@ -990,7 +978,7 @@
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
       <c r="C12" s="25" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="26"/>
@@ -998,7 +986,7 @@
       <c r="G12" s="27"/>
       <c r="H12" s="24"/>
       <c r="I12" s="18" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,7 +998,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E13" s="15">
         <v>42780</v>
@@ -1035,7 +1023,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E14" s="15">
         <v>42781</v>
@@ -1058,7 +1046,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E15" s="15">
         <v>42782</v>
@@ -1083,7 +1071,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E16" s="15">
         <v>42781</v>
@@ -1108,7 +1096,7 @@
         <v>33</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E17" s="15">
         <v>42782</v>
@@ -1120,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="I17" s="4"/>
     </row>
@@ -1133,7 +1121,7 @@
         <v>34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E18" s="15">
         <v>42784</v>
@@ -1145,7 +1133,7 @@
         <v>0.5</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="I18" s="4"/>
     </row>
@@ -1155,16 +1143,16 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="11" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E19" s="15">
         <v>42787</v>
       </c>
       <c r="F19" s="15">
-        <v>42790</v>
+        <v>42787</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="6">
@@ -1173,21 +1161,25 @@
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4">
+        <v>16</v>
+      </c>
       <c r="B20" s="4"/>
       <c r="C20" s="11" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E20" s="15">
         <v>42790</v>
       </c>
       <c r="F20" s="15">
-        <v>42796</v>
-      </c>
-      <c r="G20" s="4"/>
+        <v>42790</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
       <c r="H20" s="6"/>
       <c r="I20" s="4"/>
     </row>
@@ -1195,7 +1187,7 @@
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="21"/>
@@ -1203,71 +1195,66 @@
       <c r="G21" s="19"/>
       <c r="H21" s="22"/>
       <c r="I21" s="29" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>16</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="15">
-        <v>42791</v>
-      </c>
-      <c r="F22" s="15">
+        <v>17</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="38">
+        <v>42793</v>
+      </c>
+      <c r="F22" s="38">
         <v>42794</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="6">
-        <v>15</v>
-      </c>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="12" t="s">
-        <v>37</v>
+      <c r="C23" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E23" s="15">
-        <v>42796</v>
+        <v>42794</v>
       </c>
       <c r="F23" s="15">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="H23" s="6"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="17" t="s">
-        <v>39</v>
+      <c r="C24" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E24" s="15">
-        <v>42796</v>
+        <v>46446</v>
       </c>
       <c r="F24" s="15">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="6"/>
@@ -1275,106 +1262,92 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="11" t="s">
-        <v>38</v>
+      <c r="C25" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E25" s="15">
-        <v>42798</v>
+        <v>42797</v>
       </c>
       <c r="F25" s="15">
-        <v>42798</v>
+        <v>42801</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="6">
-        <v>18</v>
-      </c>
+      <c r="H25" s="6"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E26" s="15">
+        <v>42801</v>
+      </c>
+      <c r="F26" s="15">
+        <v>42804</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>22</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="15">
         <v>42798</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F27" s="15">
         <v>42798</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="6">
-        <v>19</v>
-      </c>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
-        <v>21</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="16">
-        <v>42800</v>
-      </c>
-      <c r="F27" s="16">
-        <v>42800</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="8">
-        <v>20</v>
-      </c>
-      <c r="I27" s="7"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28" s="7"/>
-      <c r="C28" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="C28" s="13"/>
       <c r="D28" s="7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E28" s="16">
-        <v>42801</v>
+        <v>42800</v>
       </c>
       <c r="F28" s="16">
-        <v>42801</v>
+        <v>42800</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="8">
-        <v>21</v>
-      </c>
+      <c r="H28" s="8"/>
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B29" s="7"/>
-      <c r="C29" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="C29" s="13"/>
       <c r="D29" s="7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E29" s="16">
         <v>42801</v>
@@ -1383,94 +1356,94 @@
         <v>42801</v>
       </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="8">
-        <v>22</v>
-      </c>
+      <c r="H29" s="8"/>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" s="7"/>
-      <c r="C30" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="C30" s="13"/>
       <c r="D30" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E30" s="16">
+        <v>42801</v>
+      </c>
+      <c r="F30" s="16">
+        <v>42801</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>26</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="16">
         <v>42803</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F31" s="16">
         <v>42805</v>
       </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8">
-        <v>15</v>
-      </c>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>25</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="15">
-        <v>42807</v>
-      </c>
-      <c r="F31" s="15">
-        <v>42808</v>
-      </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="6">
-        <v>24</v>
-      </c>
-      <c r="I31" s="4"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="14" t="s">
-        <v>45</v>
-      </c>
+      <c r="C32" s="13"/>
       <c r="D32" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E32" s="15">
-        <v>42810</v>
+        <v>42807</v>
       </c>
       <c r="F32" s="15">
-        <v>42812</v>
+        <v>42808</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="6">
-        <v>16</v>
-      </c>
+      <c r="H32" s="6"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="15">
+        <v>42810</v>
+      </c>
+      <c r="F33" s="15">
+        <v>42812</v>
+      </c>
       <c r="G33" s="4"/>
       <c r="H33" s="6"/>
       <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Minor Changes in UI
</commit_message>
<xml_diff>
--- a/Documentation/QUALITY/SQA Checklist.xlsx
+++ b/Documentation/QUALITY/SQA Checklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Task ID</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>End-user Web Application</t>
+  </si>
+  <si>
+    <t>Cost Analysis</t>
   </si>
 </sst>
 </file>
@@ -400,22 +403,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:F29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,30 +716,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1202,19 +1205,19 @@
       <c r="A22" s="4">
         <v>17</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="34">
         <v>42793</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="34">
         <v>42794</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="33">
         <v>1</v>
       </c>
     </row>
@@ -1235,7 +1238,9 @@
       <c r="F23" s="15">
         <v>42797</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="5">
+        <v>0.8</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="4"/>
     </row>
@@ -1251,12 +1256,14 @@
         <v>41</v>
       </c>
       <c r="E24" s="15">
-        <v>46446</v>
+        <v>42796</v>
       </c>
       <c r="F24" s="15">
-        <v>42797</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>42801</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.2</v>
+      </c>
       <c r="H24" s="6"/>
       <c r="I24" s="4"/>
     </row>
@@ -1286,91 +1293,77 @@
         <v>21</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="11" t="s">
-        <v>55</v>
+      <c r="C26" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E26" s="15">
-        <v>42801</v>
+        <v>42798</v>
       </c>
       <c r="F26" s="15">
-        <v>42804</v>
+        <v>42798</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="6"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="4">
         <v>22</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="D27" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E27" s="15">
-        <v>42798</v>
+        <v>42801</v>
       </c>
       <c r="F27" s="15">
-        <v>42798</v>
+        <v>42804</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="6"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>23</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="16">
-        <v>42800</v>
-      </c>
-      <c r="F28" s="16">
-        <v>42800</v>
-      </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15">
+        <v>42798</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
-        <v>24</v>
-      </c>
+      <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="16">
-        <v>42801</v>
-      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="16">
-        <v>42801</v>
+        <v>42800</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
-        <v>25</v>
-      </c>
+      <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="16">
-        <v>42801</v>
-      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="16"/>
       <c r="F30" s="16">
         <v>42801</v>
       </c>
@@ -1379,71 +1372,66 @@
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>26</v>
-      </c>
+      <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="13"/>
-      <c r="D31" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="16">
-        <v>42803</v>
-      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="16">
-        <v>42805</v>
+        <v>42801</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="8"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>27</v>
-      </c>
-      <c r="B32" s="4"/>
+    <row r="32" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="13"/>
-      <c r="D32" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="15">
-        <v>42807</v>
-      </c>
-      <c r="F32" s="15">
+      <c r="D32" s="7"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16">
+        <v>42805</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15">
         <v>42808</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>28</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="15">
-        <v>42810</v>
-      </c>
-      <c r="F33" s="15">
-        <v>42812</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="6"/>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="14"/>
       <c r="D34" s="4"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+      <c r="F34" s="15">
+        <v>42812</v>
+      </c>
       <c r="G34" s="4"/>
       <c r="H34" s="6"/>
       <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>